<commit_message>
Offline ESPN .CSV's Added
Updates to Scrum Board Excel as well
</commit_message>
<xml_diff>
--- a/Scrum_Board.xlsx
+++ b/Scrum_Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="940" windowWidth="37680" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="37680" windowHeight="18020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>In Progress</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Store and retrieve data from server</t>
+  </si>
+  <si>
+    <t>Research and get working example of multithreading</t>
   </si>
 </sst>
 </file>
@@ -220,8 +223,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,7 +312,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -273,6 +320,28 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -280,6 +349,28 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,11 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="A17:XFD17"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -675,6 +766,9 @@
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
@@ -686,146 +780,186 @@
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="H4" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="1:9" ht="32" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="32" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="31" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="31" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="45">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:7" ht="30">
+      <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="30">
-      <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="30">
       <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30">
+      <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:7" ht="45">
+      <c r="A24" s="2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30">
-      <c r="A24" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30">
       <c r="A26" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30">
+      <c r="A27" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>